<commit_message>
fix get product for petayer
</commit_message>
<xml_diff>
--- a/database/industries/folad/folad/income/quarterly/rial.xlsx
+++ b/database/industries/folad/folad/income/quarterly/rial.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="e:\Trade\database\industries\folad\folad\income\quarterly\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Trade\database\industries\folad\folad\income\quarterly\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1609812D-68FE-4457-B7EC-E619EA80CAF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2652" yWindow="2652" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2655" yWindow="2655" windowWidth="17280" windowHeight="8970"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -154,8 +153,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF333333"/>
@@ -189,6 +192,11 @@
       <sz val="11"/>
       <color rgb="FF333333"/>
       <name val="Calibri Bold"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="5">
@@ -251,10 +259,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -301,8 +310,12 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -614,12 +627,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:M28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="J1" activePane="topRight" state="frozen"/>
+      <selection activeCell="A7" sqref="A7"/>
+      <selection pane="topRight" activeCell="L26" sqref="L26"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="54" customWidth="1"/>
     <col min="3" max="3" width="5" customWidth="1"/>
@@ -630,7 +647,7 @@
     <col min="12" max="13" width="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -644,7 +661,7 @@
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
     </row>
-    <row r="2" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -660,7 +677,7 @@
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
     </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
@@ -676,7 +693,7 @@
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -690,7 +707,7 @@
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
     </row>
-    <row r="5" spans="2:13" ht="40.799999999999997" x14ac:dyDescent="0.75">
+    <row r="5" spans="2:13" ht="42" x14ac:dyDescent="0.65">
       <c r="B5" s="4" t="s">
         <v>2</v>
       </c>
@@ -706,7 +723,7 @@
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
     </row>
-    <row r="6" spans="2:13" ht="40.799999999999997" x14ac:dyDescent="0.75">
+    <row r="6" spans="2:13" ht="42" x14ac:dyDescent="0.65">
       <c r="B6" s="5" t="s">
         <v>3</v>
       </c>
@@ -722,7 +739,7 @@
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -736,7 +753,7 @@
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
     </row>
-    <row r="8" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="7" t="s">
         <v>4</v>
       </c>
@@ -772,7 +789,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B9" s="8" t="s">
         <v>15</v>
       </c>
@@ -808,7 +825,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B10" s="10"/>
       <c r="C10" s="11"/>
       <c r="D10" s="11"/>
@@ -822,7 +839,7 @@
       <c r="L10" s="11"/>
       <c r="M10" s="11"/>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B11" s="12" t="s">
         <v>26</v>
       </c>
@@ -858,7 +875,7 @@
         <v>322064856</v>
       </c>
     </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B12" s="10" t="s">
         <v>27</v>
       </c>
@@ -894,7 +911,7 @@
         <v>-199337326</v>
       </c>
     </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B13" s="14" t="s">
         <v>28</v>
       </c>
@@ -930,7 +947,7 @@
         <v>122727530</v>
       </c>
     </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B14" s="10" t="s">
         <v>29</v>
       </c>
@@ -966,7 +983,7 @@
         <v>-9215101</v>
       </c>
     </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B15" s="12" t="s">
         <v>30</v>
       </c>
@@ -1002,7 +1019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B16" s="10" t="s">
         <v>31</v>
       </c>
@@ -1038,7 +1055,7 @@
         <v>3236076</v>
       </c>
     </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B17" s="14" t="s">
         <v>32</v>
       </c>
@@ -1074,7 +1091,7 @@
         <v>116748505</v>
       </c>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B18" s="10" t="s">
         <v>33</v>
       </c>
@@ -1110,7 +1127,7 @@
         <v>-6328807</v>
       </c>
     </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B19" s="12" t="s">
         <v>34</v>
       </c>
@@ -1146,7 +1163,7 @@
         <v>23264642</v>
       </c>
     </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B20" s="16" t="s">
         <v>35</v>
       </c>
@@ -1182,7 +1199,7 @@
         <v>133684340</v>
       </c>
     </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B21" s="12" t="s">
         <v>36</v>
       </c>
@@ -1218,7 +1235,7 @@
         <v>-18189666</v>
       </c>
     </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B22" s="16" t="s">
         <v>37</v>
       </c>
@@ -1254,7 +1271,7 @@
         <v>115494674</v>
       </c>
     </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B23" s="12" t="s">
         <v>38</v>
       </c>
@@ -1290,7 +1307,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B24" s="16" t="s">
         <v>39</v>
       </c>
@@ -1326,7 +1343,7 @@
         <v>115494674</v>
       </c>
     </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B25" s="12" t="s">
         <v>40</v>
       </c>
@@ -1362,7 +1379,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B26" s="10" t="s">
         <v>41</v>
       </c>
@@ -1388,17 +1405,17 @@
       <c r="J26" s="11">
         <v>293000000</v>
       </c>
-      <c r="K26" s="11">
+      <c r="K26" s="18">
         <v>293000000</v>
       </c>
-      <c r="L26" s="11">
+      <c r="L26" s="18">
         <v>293000000</v>
       </c>
-      <c r="M26" s="11">
-        <v>293000000</v>
-      </c>
-    </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="M26" s="18">
+        <v>530000000</v>
+      </c>
+    </row>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B27" s="12" t="s">
         <v>42</v>
       </c>
@@ -1434,7 +1451,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>

</xml_diff>